<commit_message>
Updated readme and C6 value
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Documents\GitHub\ESP32-SensorNode\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC5A0D9-AF5D-4E93-AFEC-967B9A842112}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C845D5E1-3A50-42EC-9458-314A1C9B0A98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="503" windowWidth="20715" windowHeight="13274" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,18 +39,12 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>C1,C2</t>
-  </si>
-  <si>
     <t>CL10A226MQ8NRNC</t>
   </si>
   <si>
     <t>22uF</t>
   </si>
   <si>
-    <t>C6,C8,C11,C13</t>
-  </si>
-  <si>
     <t>CL10A475KQ8NNND</t>
   </si>
   <si>
@@ -238,6 +232,12 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>C8,C11,C13</t>
+  </si>
+  <si>
+    <t>C1,C2,C6</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
@@ -632,19 +632,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="F3" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
@@ -652,19 +652,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
@@ -672,19 +672,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F5" s="2">
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
@@ -692,17 +692,17 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.45">
@@ -710,17 +710,17 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2">
         <v>3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.45">
@@ -728,17 +728,17 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2">
         <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
@@ -746,17 +746,17 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
@@ -764,17 +764,17 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
@@ -782,17 +782,17 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2">
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
@@ -800,17 +800,17 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2">
         <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.45">
@@ -818,19 +818,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="F13" s="2">
         <v>4</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
@@ -838,19 +838,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F14" s="2">
         <v>5</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
@@ -858,19 +858,19 @@
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="F15" s="2">
         <v>5</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
@@ -878,17 +878,17 @@
         <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
@@ -896,17 +896,17 @@
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
@@ -914,17 +914,17 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
@@ -932,17 +932,17 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.45">
@@ -950,17 +950,17 @@
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
@@ -968,17 +968,17 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
@@ -987,14 +987,14 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>